<commit_message>
updating the generator profiles to more realistic characteristics
</commit_message>
<xml_diff>
--- a/ESG-Analysis/ESGPorfolios_CapacityExpansion.xlsx
+++ b/ESG-Analysis/ESGPorfolios_CapacityExpansion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A\Box\EEP147\2024\ESG\Datahub\EEP-147-SP24\ESG-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E351171-2289-44C0-BA0D-DEA2CBFF1AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7141D5A-F37A-401F-A140-E097B7F88117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="0" windowWidth="41700" windowHeight="20985" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-53" yWindow="-53" windowWidth="25706" windowHeight="15386" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ESGPorfolios_CapacityExpansion" sheetId="1" r:id="rId1"/>
@@ -631,7 +631,7 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>